<commit_message>
excel out txt in
</commit_message>
<xml_diff>
--- a/wordList.xlsx
+++ b/wordList.xlsx
@@ -5829,9 +5829,6 @@
       <c r="B67" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C67" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row customHeight="1" ht="15.75" r="68" spans="1:3" thickBot="1">
       <c r="A68" s="4" t="s">
@@ -6440,7 +6437,7 @@
         <v>263</v>
       </c>
       <c r="C141" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:3">
@@ -6980,9 +6977,6 @@
       <c r="B203" s="3" t="s">
         <v>380</v>
       </c>
-      <c r="C203" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="204" spans="1:3">
       <c r="A204" s="3" t="s">
@@ -6991,9 +6985,6 @@
       <c r="B204" s="3" t="s">
         <v>382</v>
       </c>
-      <c r="C204" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="205" spans="1:3">
       <c r="A205" s="3" t="s">
@@ -7002,9 +6993,6 @@
       <c r="B205" s="3" t="s">
         <v>384</v>
       </c>
-      <c r="C205" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="206" spans="1:3">
       <c r="A206" s="3" t="s">
@@ -7013,9 +7001,6 @@
       <c r="B206" s="3" t="s">
         <v>386</v>
       </c>
-      <c r="C206" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="207" spans="1:3">
       <c r="A207" s="3" t="s">
@@ -7024,9 +7009,6 @@
       <c r="B207" s="3" t="s">
         <v>388</v>
       </c>
-      <c r="C207" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="208" spans="1:3">
       <c r="A208" s="3" t="s">
@@ -7035,9 +7017,6 @@
       <c r="B208" s="3" t="s">
         <v>390</v>
       </c>
-      <c r="C208" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="209" spans="1:3">
       <c r="A209" s="3" t="s">
@@ -7046,9 +7025,6 @@
       <c r="B209" s="3" t="s">
         <v>392</v>
       </c>
-      <c r="C209" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="210" spans="1:3">
       <c r="A210" s="3" t="s">
@@ -7057,9 +7033,6 @@
       <c r="B210" s="3" t="s">
         <v>394</v>
       </c>
-      <c r="C210" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="211" spans="1:3">
       <c r="A211" s="3" t="s">
@@ -7068,9 +7041,6 @@
       <c r="B211" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="C211" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="212" spans="1:3">
       <c r="A212" s="3" t="s">
@@ -7079,9 +7049,6 @@
       <c r="B212" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="C212" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="213" spans="1:3">
       <c r="A213" s="3" t="s">
@@ -7090,9 +7057,6 @@
       <c r="B213" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="C213" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="214" spans="1:3">
       <c r="A214" s="3" t="s">
@@ -7101,9 +7065,6 @@
       <c r="B214" s="3" t="s">
         <v>402</v>
       </c>
-      <c r="C214" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="215" spans="1:3">
       <c r="A215" s="3" t="s">
@@ -7112,9 +7073,6 @@
       <c r="B215" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="C215" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="216" spans="1:3">
       <c r="A216" s="3" t="s">
@@ -7123,9 +7081,6 @@
       <c r="B216" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="C216" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="217" spans="1:3">
       <c r="A217" s="3" t="s">
@@ -7134,9 +7089,6 @@
       <c r="B217" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="C217" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="218" spans="1:3">
       <c r="A218" s="3" t="s">
@@ -7145,9 +7097,6 @@
       <c r="B218" s="3" t="s">
         <v>409</v>
       </c>
-      <c r="C218" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="219" spans="1:3">
       <c r="A219" s="3" t="s">
@@ -7156,9 +7105,6 @@
       <c r="B219" s="3" t="s">
         <v>411</v>
       </c>
-      <c r="C219" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="220" spans="1:3">
       <c r="A220" s="3" t="s">
@@ -7168,7 +7114,7 @@
         <v>412</v>
       </c>
       <c r="C220" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="221" spans="1:3">
@@ -7178,9 +7124,6 @@
       <c r="B221" s="3" t="s">
         <v>414</v>
       </c>
-      <c r="C221" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="222" spans="1:3">
       <c r="A222" s="3" t="s">
@@ -7190,7 +7133,7 @@
         <v>416</v>
       </c>
       <c r="C222" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="223" spans="1:3">
@@ -7200,9 +7143,6 @@
       <c r="B223" s="3" t="s">
         <v>417</v>
       </c>
-      <c r="C223" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="224" spans="1:3">
       <c r="A224" s="3" t="s">
@@ -7212,7 +7152,7 @@
         <v>419</v>
       </c>
       <c r="C224" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:3">
@@ -7222,9 +7162,6 @@
       <c r="B225" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="C225" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="226" spans="1:3">
       <c r="A226" s="3" t="s">
@@ -7233,9 +7170,6 @@
       <c r="B226" s="3" t="s">
         <v>423</v>
       </c>
-      <c r="C226" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="227" spans="1:3">
       <c r="A227" s="3" t="s">
@@ -7244,9 +7178,6 @@
       <c r="B227" s="3" t="s">
         <v>425</v>
       </c>
-      <c r="C227" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="228" spans="1:3">
       <c r="A228" s="3" t="s">
@@ -7255,9 +7186,6 @@
       <c r="B228" s="3" t="s">
         <v>427</v>
       </c>
-      <c r="C228" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="229" spans="1:3">
       <c r="A229" s="3" t="s">
@@ -7266,9 +7194,6 @@
       <c r="B229" s="3" t="s">
         <v>429</v>
       </c>
-      <c r="C229" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="230" spans="1:3">
       <c r="A230" s="3" t="s">
@@ -7277,9 +7202,6 @@
       <c r="B230" s="3" t="s">
         <v>431</v>
       </c>
-      <c r="C230" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="231" spans="1:3">
       <c r="A231" s="3" t="s">
@@ -7288,9 +7210,6 @@
       <c r="B231" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="C231" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="232" spans="1:3">
       <c r="A232" s="3" t="s">
@@ -7299,9 +7218,6 @@
       <c r="B232" s="3" t="s">
         <v>435</v>
       </c>
-      <c r="C232" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="233" spans="1:3">
       <c r="A233" s="3" t="s">
@@ -7310,9 +7226,6 @@
       <c r="B233" s="3" t="s">
         <v>437</v>
       </c>
-      <c r="C233" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="234" spans="1:3">
       <c r="A234" s="3" t="s">
@@ -7321,9 +7234,6 @@
       <c r="B234" s="3" t="s">
         <v>439</v>
       </c>
-      <c r="C234" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="235" spans="1:3">
       <c r="A235" s="3" t="s">
@@ -7332,9 +7242,6 @@
       <c r="B235" s="3" t="s">
         <v>441</v>
       </c>
-      <c r="C235" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="236" spans="1:3">
       <c r="A236" s="3" t="s">
@@ -7343,9 +7250,6 @@
       <c r="B236" s="3" t="s">
         <v>443</v>
       </c>
-      <c r="C236" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="237" spans="1:3">
       <c r="A237" s="3" t="s">
@@ -7354,9 +7258,6 @@
       <c r="B237" s="3" t="s">
         <v>445</v>
       </c>
-      <c r="C237" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="238" spans="1:3">
       <c r="A238" s="3" t="s">
@@ -7365,9 +7266,6 @@
       <c r="B238" s="3" t="s">
         <v>447</v>
       </c>
-      <c r="C238" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="239" spans="1:3">
       <c r="A239" s="3" t="s">
@@ -7376,9 +7274,6 @@
       <c r="B239" s="3" t="s">
         <v>449</v>
       </c>
-      <c r="C239" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row customHeight="1" ht="24" r="240" spans="1:3">
       <c r="A240" s="3" t="s">
@@ -7388,7 +7283,7 @@
         <v>451</v>
       </c>
       <c r="C240" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="241" spans="1:3">
@@ -7398,9 +7293,6 @@
       <c r="B241" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="C241" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="242" spans="1:3">
       <c r="A242" s="3" t="s">
@@ -7410,7 +7302,7 @@
         <v>455</v>
       </c>
       <c r="C242" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="243" spans="1:3">
@@ -7420,9 +7312,6 @@
       <c r="B243" s="3" t="s">
         <v>457</v>
       </c>
-      <c r="C243" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="244" spans="1:3">
       <c r="A244" s="3" t="s">
@@ -7431,9 +7320,6 @@
       <c r="B244" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="C244" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="245" spans="1:3">
       <c r="A245" s="3" t="s">
@@ -7442,9 +7328,6 @@
       <c r="B245" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="C245" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="246" spans="1:3">
       <c r="A246" s="3" t="s">
@@ -7453,9 +7336,6 @@
       <c r="B246" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="C246" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="247" spans="1:3">
       <c r="A247" s="3" t="s">
@@ -7464,9 +7344,6 @@
       <c r="B247" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="C247" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="248" spans="1:3">
       <c r="A248" s="3" t="s">
@@ -7475,9 +7352,6 @@
       <c r="B248" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="C248" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="249" spans="1:3">
       <c r="A249" s="3" t="s">
@@ -7486,9 +7360,6 @@
       <c r="B249" s="3" t="s">
         <v>469</v>
       </c>
-      <c r="C249" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="250" spans="1:3">
       <c r="A250" s="3" t="s">
@@ -7497,9 +7368,6 @@
       <c r="B250" s="3" t="s">
         <v>471</v>
       </c>
-      <c r="C250" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="251" spans="1:3">
       <c r="A251" s="3" t="s">
@@ -7508,9 +7376,6 @@
       <c r="B251" s="3" t="s">
         <v>473</v>
       </c>
-      <c r="C251" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="252" spans="1:3">
       <c r="A252" s="3" t="s">
@@ -7519,9 +7384,6 @@
       <c r="B252" s="3" t="s">
         <v>475</v>
       </c>
-      <c r="C252" t="n">
-        <v>1</v>
-      </c>
     </row>
     <row r="253" spans="1:3">
       <c r="A253" s="3" t="s">
@@ -8811,7 +8673,7 @@
         <v>743</v>
       </c>
       <c r="C392" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="393" spans="1:3">
@@ -8855,7 +8717,7 @@
         <v>751</v>
       </c>
       <c r="C396" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="397" spans="1:3">
@@ -9031,7 +8893,7 @@
         <v>781</v>
       </c>
       <c r="C412" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="413" spans="1:3">
@@ -9075,7 +8937,7 @@
         <v>789</v>
       </c>
       <c r="C416" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="417" spans="1:3">

</xml_diff>